<commit_message>
More complete build of EVE component of project
</commit_message>
<xml_diff>
--- a/tabular/eve/ebv-refcon-data.xlsx
+++ b/tabular/eve/ebv-refcon-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/RNA-ve/Bornaviridae-GLUE/tabular/eve/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/RNA-ve/Bornaviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C8DC65-D08D-2F4B-B2E1-77DFB90BF501}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C80729-454E-6146-9414-0F425FD0C4A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11580" yWindow="5460" windowWidth="28040" windowHeight="17440" xr2:uid="{653F5C6D-012C-DC4C-9937-8E62A09E8E67}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>EBLN-1</t>
   </si>
@@ -47,13 +47,22 @@
     <t>EBLN-4</t>
   </si>
   <si>
-    <t>EBLG-1</t>
-  </si>
-  <si>
-    <t>fullname</t>
-  </si>
-  <si>
-    <t>element_ID</t>
+    <t>sequenceID</t>
+  </si>
+  <si>
+    <t>virus_full_name</t>
+  </si>
+  <si>
+    <t>virus_name</t>
+  </si>
+  <si>
+    <t>virus_family</t>
+  </si>
+  <si>
+    <t>virus_genus</t>
+  </si>
+  <si>
+    <t>virus_clade</t>
   </si>
 </sst>
 </file>
@@ -70,8 +79,8 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="14"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -86,14 +95,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="0" tint="-0.14996795556505021"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14996795556505021"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FF000090"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -111,8 +120,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B744EB1-D110-324B-95CE-A3C70BC175EB}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="A6" sqref="A6:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -438,57 +447,44 @@
     <col min="1" max="1" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>